<commit_message>
New excel export format method
</commit_message>
<xml_diff>
--- a/frontend-next/public/templates/export_template.xlsx
+++ b/frontend-next/public/templates/export_template.xlsx
@@ -22,124 +22,124 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
-    <t xml:space="preserve">Número de control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apellido paterno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apellido materno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sexo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estado de nacimiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de nacimiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carrera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Periodo de ingreso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Periodo de egreso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de título</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha del acto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan de estudios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de registro (Título)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de cédula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observaciones (Título)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de folio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de registro (certificado)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observaciones (certificado)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.num_control}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.nombre}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.apellidop}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.apellidom}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.sexo}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.estado_nacimiento}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.fecha_nacimiento}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.CURP}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.nombre_carrera}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.periodo_ingreso}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.periodo_egreso}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.num_titulo}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.fecha_acto}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.clave_plan}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.fecha_registro_tit}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.num_cedula}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.observaciones_tit}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.num_folio}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.fecha_registro_cert}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{data.observaciones_cert}</t>
+    <t xml:space="preserve">{headers.column1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{headers.column20}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column5}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column6}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column7}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column8}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column9}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column12}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column13}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column14}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column15}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column17}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column18}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column19}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{data.column20}</t>
   </si>
 </sst>
 </file>
@@ -149,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -181,6 +181,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Droid Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -193,11 +199,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Droid Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +216,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2A6099"/>
         <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -262,7 +276,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,7 +284,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,25 +474,25 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="28.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="26.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="26.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="26.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="23.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="23.96"/>
@@ -493,7 +507,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="21.83"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,122 +520,122 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>